<commit_message>
Updated comment for B12
</commit_message>
<xml_diff>
--- a/dataactvalidator/config/rule_documentation.xlsx
+++ b/dataactvalidator/config/rule_documentation.xlsx
@@ -441,9 +441,6 @@
     <t>Condtional requirement, in set</t>
   </si>
   <si>
-    <t>Unclear what the condition is</t>
-  </si>
-  <si>
     <t>Cross file existence</t>
   </si>
   <si>
@@ -460,6 +457,9 @@
   </si>
   <si>
     <t>Only 2 cross file calcs (A &amp; B), which need more explanation</t>
+  </si>
+  <si>
+    <t>Unclear what the condition is, this check is currently applied to all records</t>
   </si>
 </sst>
 </file>
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2109,7 +2109,7 @@
         <v>119</v>
       </c>
       <c r="G38" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2264,7 +2264,7 @@
         <v>99</v>
       </c>
       <c r="E46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F46" t="s">
         <v>115</v>
@@ -2284,7 +2284,7 @@
         <v>99</v>
       </c>
       <c r="E47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F47" t="s">
         <v>115</v>
@@ -2304,13 +2304,13 @@
         <v>99</v>
       </c>
       <c r="E48" t="s">
+        <v>140</v>
+      </c>
+      <c r="F48" t="s">
+        <v>119</v>
+      </c>
+      <c r="G48" t="s">
         <v>141</v>
-      </c>
-      <c r="F48" t="s">
-        <v>119</v>
-      </c>
-      <c r="G48" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -2327,13 +2327,13 @@
         <v>99</v>
       </c>
       <c r="E49" t="s">
+        <v>140</v>
+      </c>
+      <c r="F49" t="s">
+        <v>119</v>
+      </c>
+      <c r="G49" t="s">
         <v>141</v>
-      </c>
-      <c r="F49" t="s">
-        <v>119</v>
-      </c>
-      <c r="G49" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
@@ -2350,13 +2350,13 @@
         <v>109</v>
       </c>
       <c r="E50" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F50" t="s">
         <v>115</v>
       </c>
       <c r="G50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
@@ -2373,7 +2373,7 @@
         <v>109</v>
       </c>
       <c r="E51" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F51" t="s">
         <v>119</v>
@@ -2384,12 +2384,12 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>